<commit_message>
fix to pacific soil data entry sheet
</commit_message>
<xml_diff>
--- a/www/Configs/PacificSoils/Data Entry Template - PacificSoils.xlsx
+++ b/www/Configs/PacificSoils/Data Entry Template - PacificSoils.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/sea084_csiro_au/Documents/RossRCode/Git/Shiny/Apps/SoilDataEntry/www/Configs/PacificSoils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{85FB1B30-9AB1-4C64-BF2C-F6282794E71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF72F986-4A9A-433C-9BD6-4E5A667FB8C4}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{85FB1B30-9AB1-4C64-BF2C-F6282794E71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61FB56E8-6DD5-46AF-845E-8D3E569D3958}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="-17145" windowWidth="24285" windowHeight="14340" firstSheet="1" activeTab="1" xr2:uid="{83C9EC8A-7EF8-4F9D-A138-3450D8759736}"/>
+    <workbookView xWindow="5370" yWindow="-17145" windowWidth="24285" windowHeight="14340" firstSheet="4" activeTab="4" xr2:uid="{83C9EC8A-7EF8-4F9D-A138-3450D8759736}"/>
   </bookViews>
   <sheets>
     <sheet name="TemplateOriginal" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="DBInfo" sheetId="8" r:id="rId2"/>
+    <sheet name="DBInfo" sheetId="8" state="hidden" r:id="rId2"/>
     <sheet name="DBTableLevels" sheetId="9" state="hidden" r:id="rId3"/>
     <sheet name="Codes" sheetId="2" state="hidden" r:id="rId4"/>
     <sheet name="About" sheetId="13" r:id="rId5"/>
@@ -9585,7 +9585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47E6B88-97CE-436E-8F7D-17E89501757A}">
   <dimension ref="A1:AU33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -12287,6 +12287,7 @@
       <c r="Q33" s="26"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="SzjsoZlDXgVD4jopHF7t83lF7nKIauomaSe9F1KMQ8//rQIjy8QZ08MiExQHZ/8bB8rU39+v04lyk+fymIQhJQ==" saltValue="BmzsHFflk27Tx4zS57CoSQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18964,7 +18965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064B206F-F17C-4025-942F-53FBF697F5D0}">
   <dimension ref="A1:AJ56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>